<commit_message>
Add existing file 2022-08-02 09:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,12 +506,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M. Kozioł</t>
+          <t>D. Arndt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2610</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -576,12 +576,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M. Kołba</t>
+          <t>A. Bobek</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -646,12 +646,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D. Arndt</t>
+          <t>M. Kozioł</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -661,17 +661,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -716,12 +716,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A. Bobek</t>
+          <t>M. Kołba</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -786,32 +786,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>M. Kot</t>
+          <t>M. Bąkowicz</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>O</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -856,12 +856,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A. Marciniak</t>
+          <t>M. Dąbrowski</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -871,32 +871,32 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1280</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -926,12 +926,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>M. Dąbrowski</t>
+          <t>K. Dankowski</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -941,47 +941,47 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1684</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -996,12 +996,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>B. Szeliga</t>
+          <t>O. Koprowski</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1011,42 +1011,42 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2209</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>K. Dankowski</t>
+          <t>M. Lorenc</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1081,32 +1081,32 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1136,12 +1136,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nacho Monsalve</t>
+          <t>A. Marciniak</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>33</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1151,42 +1151,42 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>676</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A. Klimczak</t>
+          <t>Nacho Monsalve</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1221,32 +1221,32 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1259</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1276,12 +1276,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>J. Sobociński</t>
+          <t>B. Szeliga</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>29</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1291,42 +1291,42 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>712</t>
+          <t>256</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1346,12 +1346,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>O. Koprowski</t>
+          <t>M. Wszołek</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1361,32 +1361,32 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1786</t>
+          <t>189</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1416,47 +1416,47 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>M. Lorenc</t>
+          <t>B. Biel</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>483</t>
+          <t>217</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1486,27 +1486,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>M. Wszołek</t>
+          <t>P. Gryszkiewicz</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>M. Bąkowicz</t>
+          <t>K. Ibe-Torti</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1566,37 +1566,37 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1867</t>
+          <t>82</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>J. Tosik</t>
+          <t>D. Kort</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>27</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1641,32 +1641,32 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>830</t>
+          <t>234</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1696,12 +1696,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>M. Rygaard</t>
+          <t>M. Kowalczyk</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1711,32 +1711,32 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>643</t>
+          <t>125</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ricardinho</t>
+          <t>J. Kuźma</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1781,32 +1781,32 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1095</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1836,12 +1836,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Antonio Domínguez</t>
+          <t>Javi Moreno</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1851,42 +1851,42 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1507</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1906,12 +1906,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>M. Trąbka</t>
+          <t>D. Nowacki</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1921,17 +1921,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2113</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1951,12 +1951,12 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1976,12 +1976,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>M. Rozwandowicz</t>
+          <t>V. Okhronchuk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1991,42 +1991,42 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1522</t>
+          <t>116</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>9</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2046,12 +2046,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>D. Nowacki</t>
+          <t>J. Romanowicz</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2061,12 +2061,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2116,12 +2116,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>J. Kuźma</t>
+          <t>Pirulo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2131,42 +2131,42 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>270</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2186,12 +2186,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P. Gryszkiewicz</t>
+          <t>M. Trąbka</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2201,32 +2201,32 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>262</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2256,57 +2256,57 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>M. Kowalczyk</t>
+          <t>N. Balongo</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>230</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Pirulo</t>
+          <t>P. Janczukowicz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2341,17 +2341,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2619</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2361,22 +2361,22 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2396,12 +2396,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Javi Moreno</t>
+          <t>J. Piotrowski</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2411,32 +2411,32 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1612</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>M. Wolski</t>
+          <t>M. Radaszkiewicz</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2481,42 +2481,42 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1571</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2536,69 +2536,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Samu Corral</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>743</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+          <t>K. Moskal</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2606,349 +2558,21 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>S. Jurić</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>741</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>M. Radaszkiewicz</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>1102</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>P. Janczukowicz</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>688</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>K. Ibe-Torti</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>585</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>D. Gmosiński</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+          <t>M. Pogorzała</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add existing file 2022-08-07 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -1741,7 +1741,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-08 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -661,17 +661,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>360</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -941,12 +941,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>113</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>360</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1291,17 +1291,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>346</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1361,17 +1361,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>247</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1431,27 +1431,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>290</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>82</t>
+          <t>99</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>292</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1711,17 +1711,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>215</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1781,12 +1781,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>69</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>356</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>352</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2271,27 +2271,27 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>303</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2341,42 +2341,42 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>37</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-11 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -971,7 +971,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-12 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>360</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>450</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>203</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1081,12 +1081,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>450</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1291,17 +1291,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>436</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1431,22 +1431,22 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>290</t>
+          <t>317</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1571,27 +1571,27 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>162</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1711,17 +1711,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>305</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1781,27 +1781,27 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>38</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1991,32 +1991,32 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>125</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>419</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>433</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2271,22 +2271,22 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>303</t>
+          <t>321</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2341,27 +2341,27 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>109</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-15 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>450</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>540</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>293</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>540</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1291,17 +1291,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>436</t>
+          <t>526</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1431,27 +1431,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>317</t>
+          <t>372</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1571,32 +1571,32 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>162</t>
+          <t>197</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,32 +1641,32 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>292</t>
+          <t>327</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1711,42 +1711,42 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>360</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1781,17 +1781,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>215</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>47</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>150</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>419</t>
+          <t>509</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>433</t>
+          <t>514</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2271,12 +2271,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>346</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2341,17 +2341,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>174</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-23 22:53:54 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>540</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>540</t>
+          <t>630</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>383</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,17 +1011,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>104</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1081,27 +1081,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>91</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>540</t>
+          <t>630</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1431,27 +1431,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>372</t>
+          <t>434</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1571,24 +1571,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>225</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="I17" t="inlineStr">
         <is>
           <t>1</t>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,19 +1641,19 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>400</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>1</t>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1711,42 +1711,42 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>422</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1781,32 +1781,32 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>223</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>167</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2006,17 +2006,17 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>509</t>
+          <t>582</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2201,22 +2201,22 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>542</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>436</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2341,32 +2341,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>191</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-29 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>540</t>
+          <t>630</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>630</t>
+          <t>720</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>473</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,24 +1011,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>113</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>0</t>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>147</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>630</t>
+          <t>720</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1291,17 +1291,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>526</t>
+          <t>607</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1431,12 +1431,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>434</t>
+          <t>468</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1571,17 +1571,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>281</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1641,19 +1641,19 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>456</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>1</t>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1781,32 +1781,32 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>257</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
           <t>6</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>582</t>
+          <t>670</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2166,12 +2166,12 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>542</t>
+          <t>632</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>7</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>6</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>436</t>
+          <t>505</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2341,32 +2341,32 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>191</t>
+          <t>212</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-08-30 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P. Gryszkiewicz</t>
+          <t>K. Ibe-Torti</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1501,32 +1501,32 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>281</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1556,12 +1556,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>K. Ibe-Torti</t>
+          <t>D. Kort</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>27</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1571,34 +1571,34 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>281</t>
+          <t>456</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>0</t>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>D. Kort</t>
+          <t>M. Kowalczyk</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>422</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1651,17 +1651,17 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1671,12 +1671,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1696,12 +1696,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>M. Kowalczyk</t>
+          <t>J. Kuźma</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>422</t>
+          <t>257</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1721,32 +1721,32 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>J. Kuźma</t>
+          <t>Javi Moreno</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1781,17 +1781,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1801,12 +1801,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Javi Moreno</t>
+          <t>D. Nowacki</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1906,12 +1906,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>D. Nowacki</t>
+          <t>V. Okhronchuk</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1921,32 +1921,32 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>167</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1976,12 +1976,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>V. Okhronchuk</t>
+          <t>J. Romanowicz</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1991,32 +1991,32 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2046,12 +2046,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>J. Romanowicz</t>
+          <t>Pirulo</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2061,17 +2061,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>670</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2091,17 +2091,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2116,12 +2116,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pirulo</t>
+          <t>M. Trąbka</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>670</t>
+          <t>632</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2141,12 +2141,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2156,22 +2156,22 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2186,22 +2186,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>M. Trąbka</t>
+          <t>N. Balongo</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>N</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>505</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2211,27 +2211,27 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2256,12 +2256,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>N. Balongo</t>
+          <t>P. Janczukowicz</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2271,37 +2271,37 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>212</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P. Janczukowicz</t>
+          <t>M. Radaszkiewicz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2341,42 +2341,42 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2396,183 +2396,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>J. Piotrowski</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>M. Radaszkiewicz</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
           <t>K. Moskal</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>M. Pogorzała</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add existing file 2022-08-31 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>M. Radaszkiewicz</t>
+          <t>S. Jurić</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2341,12 +2341,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2396,21 +2396,91 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>M. Radaszkiewicz</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>K. Moskal</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add existing file 2022-09-06 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -1671,7 +1671,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-09-07 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>630</t>
+          <t>720</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>810</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>473</t>
+          <t>563</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,17 +1011,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>187</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>237</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>16</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>810</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>281</t>
+          <t>305</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1571,19 +1571,19 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>522</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>1</t>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1641,42 +1641,42 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>422</t>
+          <t>512</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2061,17 +2061,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>670</t>
+          <t>760</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>722</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>8</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>7</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>571</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2271,32 +2271,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>236</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
           <t>6</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-09-12 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>720</t>
+          <t>810</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>563</t>
+          <t>653</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,17 +1011,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>277</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>237</t>
+          <t>327</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1151,17 +1151,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>106</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>900</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1431,27 +1431,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>522</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>6</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>341</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>536</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1596,17 +1596,17 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>2</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>512</t>
+          <t>602</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2061,17 +2061,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>760</t>
+          <t>836</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2131,19 +2131,19 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>812</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
           <t>1</t>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>571</t>
+          <t>625</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2271,32 +2271,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>236</t>
+          <t>272</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
           <t>7</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>6</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-09-13 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>277</t>
+          <t>274</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>812</t>
+          <t>810</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2256,12 +2256,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P. Janczukowicz</t>
+          <t>G. Glapka</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2271,42 +2271,42 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>S. Jurić</t>
+          <t>P. Janczukowicz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2341,42 +2341,42 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>272</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2396,12 +2396,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>M. Radaszkiewicz</t>
+          <t>S. Jurić</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2411,12 +2411,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2466,21 +2466,91 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>M. Radaszkiewicz</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>K. Moskal</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add existing file 2022-09-14 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>M. Wszołek</t>
+          <t>A. Tutyškinas</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1361,32 +1361,32 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1416,49 +1416,49 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>B. Biel</t>
+          <t>M. Wszołek</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>O</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>247</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>0</t>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1486,12 +1486,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>K. Ibe-Torti</t>
+          <t>B. Biel</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>522</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1511,22 +1511,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1556,12 +1556,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D. Kort</t>
+          <t>K. Ibe-Torti</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1571,32 +1571,32 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>341</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1606,7 +1606,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>M. Kowalczyk</t>
+          <t>D. Kort</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>27</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>602</t>
+          <t>536</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1661,22 +1661,22 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>2</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>5</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1696,12 +1696,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>J. Kuźma</t>
+          <t>M. Kowalczyk</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1711,42 +1711,42 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>602</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>1</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Javi Moreno</t>
+          <t>J. Kuźma</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1781,27 +1781,27 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>257</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1836,12 +1836,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D. Nowacki</t>
+          <t>Javi Moreno</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1851,12 +1851,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>81</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1906,12 +1906,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>V. Okhronchuk</t>
+          <t>D. Nowacki</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1921,34 +1921,34 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="K22" t="inlineStr">
         <is>
           <t>0</t>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1976,12 +1976,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>J. Romanowicz</t>
+          <t>V. Okhronchuk</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1991,32 +1991,32 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>167</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2046,12 +2046,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pirulo</t>
+          <t>J. Romanowicz</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2061,17 +2061,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2091,17 +2091,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2116,12 +2116,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>M. Trąbka</t>
+          <t>Pirulo</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>836</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2141,37 +2141,37 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -2186,22 +2186,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>N. Balongo</t>
+          <t>M. Trąbka</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>625</t>
+          <t>810</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2211,32 +2211,32 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2256,12 +2256,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>G. Glapka</t>
+          <t>N. Balongo</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2271,32 +2271,32 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t>625</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P. Janczukowicz</t>
+          <t>G. Glapka</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>19</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2341,42 +2341,42 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2396,12 +2396,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>S. Jurić</t>
+          <t>P. Janczukowicz</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2411,42 +2411,42 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>272</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2466,12 +2466,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>M. Radaszkiewicz</t>
+          <t>S. Jurić</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2481,12 +2481,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2536,21 +2536,91 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>M. Radaszkiewicz</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>K. Moskal</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add existing file 2022-09-19 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -591,17 +591,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>90</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>900</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>653</t>
+          <t>743</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>417</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1151,27 +1151,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>185</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>990</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1361,12 +1361,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>556</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>341</t>
+          <t>352</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>607</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1711,17 +1711,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>602</t>
+          <t>692</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>186</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>915</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2201,19 +2201,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>866</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
           <t>1</t>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>625</t>
+          <t>696</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2411,32 +2411,32 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>291</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
           <t>8</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>7</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-01 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>810</t>
+          <t>856</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -591,24 +591,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>134</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
@@ -616,7 +616,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>900</t>
+          <t>990</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>743</t>
+          <t>833</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1011,17 +1011,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>274</t>
+          <t>364</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>417</t>
+          <t>507</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>1080</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1501,27 +1501,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>556</t>
+          <t>636</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>7</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>6</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1641,29 +1641,29 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>607</t>
+          <t>697</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>8</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>3</t>
@@ -1671,12 +1671,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1781,17 +1781,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>257</t>
+          <t>326</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>866</t>
+          <t>956</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>11</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>10</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2271,12 +2271,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>696</t>
+          <t>706</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2341,12 +2341,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2411,34 +2411,34 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>291</t>
+          <t>312</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
       <c r="K29" t="inlineStr">
         <is>
           <t>1</t>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2551,19 +2551,19 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>100</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H31" t="inlineStr">
         <is>
           <t>1</t>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-08 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -1251,7 +1251,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-09 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -591,17 +591,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>224</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>1080</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>833</t>
+          <t>923</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>507</t>
+          <t>597</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>206</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1166,17 +1166,17 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1149</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1361,17 +1361,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>104</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1501,27 +1501,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>636</t>
+          <t>691</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>8</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>7</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>697</t>
+          <t>787</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1991,17 +1991,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>255</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>915</t>
+          <t>1005</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2201,12 +2201,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>956</t>
+          <t>991</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2271,12 +2271,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>706</t>
+          <t>741</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2411,32 +2411,32 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>312</t>
+          <t>333</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
           <t>10</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>9</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2551,27 +2551,27 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>155</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-16 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -546,7 +546,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -591,17 +591,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>224</t>
+          <t>314</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1080</t>
+          <t>1147</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>923</t>
+          <t>1013</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>364</t>
+          <t>377</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1026,17 +1026,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>597</t>
+          <t>687</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>229</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1149</t>
+          <t>1239</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1361,27 +1361,27 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>181</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>691</t>
+          <t>707</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>396</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,17 +1641,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>787</t>
+          <t>854</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1991,12 +1991,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>278</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2131,17 +2131,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1005</t>
+          <t>1051</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>991</t>
+          <t>1081</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>741</t>
+          <t>831</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2411,17 +2411,17 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>333</t>
+          <t>407</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-24 00:05:01 CEST
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -546,7 +546,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -591,17 +591,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>314</t>
+          <t>404</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>3</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1013</t>
+          <t>1103</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>377</t>
+          <t>397</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1081,17 +1081,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>687</t>
+          <t>722</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1151,17 +1151,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>319</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1239</t>
+          <t>1329</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1291,22 +1291,22 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>607</t>
+          <t>627</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1361,17 +1361,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>271</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1501,12 +1501,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>707</t>
+          <t>709</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1921,17 +1921,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>70</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1991,17 +1991,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>278</t>
+          <t>368</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2131,22 +2131,22 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1051</t>
+          <t>1106</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>13</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -2156,12 +2156,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1081</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>831</t>
+          <t>919</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2411,37 +2411,37 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>407</t>
+          <t>477</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2481,12 +2481,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2496,7 +2496,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">

</xml_diff>

<commit_message>
Add existing file 2022-10-31 00:05:01 CET
</commit_message>
<xml_diff>
--- a/LKS.xlsx
+++ b/LKS.xlsx
@@ -546,7 +546,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -591,17 +591,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>494</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>4</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -941,17 +941,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1103</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>441</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1151,42 +1151,42 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>319</t>
+          <t>409</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1221,17 +1221,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1329</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>627</t>
+          <t>672</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1306,22 +1306,22 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1361,17 +1361,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>361</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1641,12 +1641,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>854</t>
+          <t>870</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1921,42 +1921,42 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>116</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -1991,17 +1991,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>368</t>
+          <t>458</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2131,19 +2131,19 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1106</t>
+          <t>1196</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>14</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
           <t>1</t>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2201,17 +2201,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1169</t>
+          <t>1243</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>919</t>
+          <t>964</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2411,17 +2411,17 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>477</t>
+          <t>551</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2481,37 +2481,37 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>18</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">

</xml_diff>